<commit_message>
Update Pertanggal 05 Maret 2025 12:11 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblMapper_WorkerCareerInternalToUserRole.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblMapper_WorkerCareerInternalToUserRole.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -2171,7 +2171,7 @@
             <v>164000000000155</v>
           </cell>
           <cell r="M158" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000155::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000155::bigint, 163000000000001::bigint, 111000000000011::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="159">
@@ -3524,7 +3524,7 @@
             <v>164000000000278</v>
           </cell>
           <cell r="M281" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000278::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000278::bigint, 163000000000002::bigint, 111000000000011::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="282">
@@ -6615,7 +6615,7 @@
             <v>164000000000559</v>
           </cell>
           <cell r="M562" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000559::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000559::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000004::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="563">
@@ -6714,7 +6714,7 @@
             <v>164000000000568</v>
           </cell>
           <cell r="M571" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000568::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000568::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="572">
@@ -6725,7 +6725,7 @@
             <v>164000000000569</v>
           </cell>
           <cell r="M572" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000569::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000569::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="573">
@@ -6736,7 +6736,7 @@
             <v>164000000000570</v>
           </cell>
           <cell r="M573" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000570::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000570::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="574">
@@ -6747,7 +6747,7 @@
             <v>164000000000571</v>
           </cell>
           <cell r="M574" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000571::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000571::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="575">
@@ -6758,7 +6758,7 @@
             <v>164000000000572</v>
           </cell>
           <cell r="M575" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000572::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000572::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="576">
@@ -6769,7 +6769,7 @@
             <v>164000000000573</v>
           </cell>
           <cell r="M576" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000573::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000573::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="577">
@@ -6780,7 +6780,7 @@
             <v>164000000000574</v>
           </cell>
           <cell r="M577" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000574::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000574::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="578">
@@ -6791,7 +6791,7 @@
             <v>164000000000575</v>
           </cell>
           <cell r="M578" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000575::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000575::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="579">
@@ -6802,7 +6802,7 @@
             <v>164000000000576</v>
           </cell>
           <cell r="M579" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000576::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000576::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="580">
@@ -6813,7 +6813,7 @@
             <v>164000000000577</v>
           </cell>
           <cell r="M580" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000577::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000577::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="581">
@@ -6824,7 +6824,7 @@
             <v>164000000000578</v>
           </cell>
           <cell r="M581" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000578::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000578::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="582">
@@ -6835,7 +6835,7 @@
             <v>164000000000579</v>
           </cell>
           <cell r="M582" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000579::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000579::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="583">
@@ -6846,7 +6846,7 @@
             <v>164000000000580</v>
           </cell>
           <cell r="M583" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000580::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000580::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="584">
@@ -6857,7 +6857,7 @@
             <v>164000000000581</v>
           </cell>
           <cell r="M584" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000581::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000581::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="585">
@@ -6879,7 +6879,7 @@
             <v>164000000000583</v>
           </cell>
           <cell r="M586" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000583::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000583::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="587">
@@ -6890,7 +6890,7 @@
             <v>164000000000584</v>
           </cell>
           <cell r="M587" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000584::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000584::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
         <row r="588">
@@ -6901,7 +6901,7 @@
             <v>164000000000585</v>
           </cell>
           <cell r="M588" t="str">
-            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000585::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000585::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
       </sheetData>
@@ -7204,11 +7204,11 @@
   <dimension ref="B1:H589"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C341" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D230" sqref="D230"/>
       <selection pane="topRight" activeCell="D230" sqref="D230"/>
       <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
-      <selection pane="bottomRight" activeCell="D128" sqref="D128"/>
+      <selection pane="bottomRight" activeCell="C349" sqref="C349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7216,8 +7216,7 @@
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="4" max="5" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
@@ -9763,14 +9762,16 @@
       <c r="D128" s="3">
         <v>95000000000023</v>
       </c>
-      <c r="E128" s="3"/>
+      <c r="E128" s="3">
+        <v>46000000000009</v>
+      </c>
       <c r="G128" s="15">
         <f t="shared" si="3"/>
         <v>225000000000008</v>
       </c>
       <c r="H128" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000125::bigint, 95000000000023::bigint, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000125::bigint, 95000000000023::bigint, 46000000000009::bigint);</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.2">
@@ -10342,17 +10343,15 @@
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M157, ""), "", '[1]Internal Career (Last Position)'!$C157)</f>
         <v>Fikri</v>
       </c>
-      <c r="D157" s="3">
-        <v>95000000000023</v>
-      </c>
+      <c r="D157" s="3"/>
       <c r="E157" s="3"/>
       <c r="G157" s="15">
         <f t="shared" si="5"/>
-        <v>225000000000009</v>
+        <v>225000000000008</v>
       </c>
       <c r="H157" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000154::bigint, 95000000000023::bigint, null::bigint);</v>
+        <v/>
       </c>
     </row>
     <row r="158" spans="2:8" x14ac:dyDescent="0.2">
@@ -10364,15 +10363,19 @@
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M158, ""), "", '[1]Internal Career (Last Position)'!$C158)</f>
         <v>M. Fikri Caesarandi Hasibuan</v>
       </c>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
+      <c r="D158" s="3">
+        <v>95000000000023</v>
+      </c>
+      <c r="E158" s="3">
+        <v>46000000000033</v>
+      </c>
       <c r="G158" s="15">
         <f t="shared" si="5"/>
         <v>225000000000009</v>
       </c>
       <c r="H158" s="16" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000155::bigint, 95000000000023::bigint, 46000000000033::bigint);</v>
       </c>
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.2">
@@ -11915,14 +11918,16 @@
       <c r="D235" s="3">
         <v>95000000000018</v>
       </c>
-      <c r="E235" s="3"/>
+      <c r="E235" s="3">
+        <v>46000000000033</v>
+      </c>
       <c r="G235" s="15">
         <f t="shared" si="7"/>
         <v>225000000000014</v>
       </c>
       <c r="H235" s="16" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000232::bigint, 95000000000018::bigint, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000232::bigint, 95000000000018::bigint, 46000000000033::bigint);</v>
       </c>
     </row>
     <row r="236" spans="2:8" x14ac:dyDescent="0.2">
@@ -12838,15 +12843,19 @@
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M281, ""), "", '[1]Internal Career (Last Position)'!$C281)</f>
         <v>T. Marungkil U. S. Sagala</v>
       </c>
-      <c r="D281" s="3"/>
-      <c r="E281" s="3"/>
+      <c r="D281" s="3">
+        <v>95000000000018</v>
+      </c>
+      <c r="E281" s="3">
+        <v>46000000000009</v>
+      </c>
       <c r="G281" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H281" s="16" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000278::bigint, 95000000000018::bigint, 46000000000009::bigint);</v>
       </c>
     </row>
     <row r="282" spans="2:8" x14ac:dyDescent="0.2">
@@ -12862,7 +12871,7 @@
       <c r="E282" s="3"/>
       <c r="G282" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H282" s="16" t="str">
         <f t="shared" si="10"/>
@@ -12882,7 +12891,7 @@
       <c r="E283" s="3"/>
       <c r="G283" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H283" s="16" t="str">
         <f t="shared" si="10"/>
@@ -12902,7 +12911,7 @@
       <c r="E284" s="3"/>
       <c r="G284" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H284" s="16" t="str">
         <f t="shared" si="10"/>
@@ -12922,7 +12931,7 @@
       <c r="E285" s="3"/>
       <c r="G285" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H285" s="16" t="str">
         <f t="shared" si="10"/>
@@ -12942,7 +12951,7 @@
       <c r="E286" s="3"/>
       <c r="G286" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H286" s="16" t="str">
         <f t="shared" si="10"/>
@@ -12962,7 +12971,7 @@
       <c r="E287" s="3"/>
       <c r="G287" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H287" s="16" t="str">
         <f t="shared" si="10"/>
@@ -12982,7 +12991,7 @@
       <c r="E288" s="3"/>
       <c r="G288" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H288" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13002,7 +13011,7 @@
       <c r="E289" s="3"/>
       <c r="G289" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H289" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13022,7 +13031,7 @@
       <c r="E290" s="3"/>
       <c r="G290" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H290" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13042,7 +13051,7 @@
       <c r="E291" s="3"/>
       <c r="G291" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H291" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13062,7 +13071,7 @@
       <c r="E292" s="3"/>
       <c r="G292" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H292" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13082,7 +13091,7 @@
       <c r="E293" s="3"/>
       <c r="G293" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H293" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13102,7 +13111,7 @@
       <c r="E294" s="3"/>
       <c r="G294" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H294" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13122,7 +13131,7 @@
       <c r="E295" s="3"/>
       <c r="G295" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H295" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13142,7 +13151,7 @@
       <c r="E296" s="3"/>
       <c r="G296" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H296" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13162,7 +13171,7 @@
       <c r="E297" s="3"/>
       <c r="G297" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H297" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13182,7 +13191,7 @@
       <c r="E298" s="3"/>
       <c r="G298" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H298" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13202,7 +13211,7 @@
       <c r="E299" s="3"/>
       <c r="G299" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H299" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13222,7 +13231,7 @@
       <c r="E300" s="3"/>
       <c r="G300" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H300" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13242,7 +13251,7 @@
       <c r="E301" s="3"/>
       <c r="G301" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H301" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13262,7 +13271,7 @@
       <c r="E302" s="3"/>
       <c r="G302" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H302" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13282,7 +13291,7 @@
       <c r="E303" s="3"/>
       <c r="G303" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000016</v>
+        <v>225000000000017</v>
       </c>
       <c r="H303" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13304,7 +13313,7 @@
       <c r="E304" s="3"/>
       <c r="G304" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H304" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13324,7 +13333,7 @@
       <c r="E305" s="3"/>
       <c r="G305" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H305" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13344,7 +13353,7 @@
       <c r="E306" s="3"/>
       <c r="G306" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H306" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13364,7 +13373,7 @@
       <c r="E307" s="3"/>
       <c r="G307" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H307" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13384,7 +13393,7 @@
       <c r="E308" s="3"/>
       <c r="G308" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H308" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13404,7 +13413,7 @@
       <c r="E309" s="3"/>
       <c r="G309" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H309" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13424,7 +13433,7 @@
       <c r="E310" s="3"/>
       <c r="G310" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H310" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13444,7 +13453,7 @@
       <c r="E311" s="3"/>
       <c r="G311" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H311" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13464,7 +13473,7 @@
       <c r="E312" s="3"/>
       <c r="G312" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H312" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13484,7 +13493,7 @@
       <c r="E313" s="3"/>
       <c r="G313" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H313" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13504,7 +13513,7 @@
       <c r="E314" s="3"/>
       <c r="G314" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H314" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13524,7 +13533,7 @@
       <c r="E315" s="3"/>
       <c r="G315" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H315" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13544,7 +13553,7 @@
       <c r="E316" s="3"/>
       <c r="G316" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H316" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13564,7 +13573,7 @@
       <c r="E317" s="3"/>
       <c r="G317" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H317" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13584,7 +13593,7 @@
       <c r="E318" s="3"/>
       <c r="G318" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H318" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13604,7 +13613,7 @@
       <c r="E319" s="3"/>
       <c r="G319" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H319" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13624,7 +13633,7 @@
       <c r="E320" s="3"/>
       <c r="G320" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H320" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13644,7 +13653,7 @@
       <c r="E321" s="3"/>
       <c r="G321" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H321" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13664,7 +13673,7 @@
       <c r="E322" s="3"/>
       <c r="G322" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H322" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13684,7 +13693,7 @@
       <c r="E323" s="3"/>
       <c r="G323" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H323" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13704,7 +13713,7 @@
       <c r="E324" s="3"/>
       <c r="G324" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H324" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13724,7 +13733,7 @@
       <c r="E325" s="3"/>
       <c r="G325" s="15">
         <f t="shared" si="9"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H325" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13744,7 +13753,7 @@
       <c r="E326" s="3"/>
       <c r="G326" s="15">
         <f t="shared" ref="G326:G389" si="11" xml:space="preserve"> G325 + IF(EXACT(H326, ""), 0, 1)</f>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H326" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13764,7 +13773,7 @@
       <c r="E327" s="3"/>
       <c r="G327" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H327" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13784,7 +13793,7 @@
       <c r="E328" s="3"/>
       <c r="G328" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H328" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13804,7 +13813,7 @@
       <c r="E329" s="3"/>
       <c r="G329" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H329" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13824,7 +13833,7 @@
       <c r="E330" s="3"/>
       <c r="G330" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H330" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13844,7 +13853,7 @@
       <c r="E331" s="3"/>
       <c r="G331" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H331" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13864,7 +13873,7 @@
       <c r="E332" s="3"/>
       <c r="G332" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H332" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13884,7 +13893,7 @@
       <c r="E333" s="3"/>
       <c r="G333" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H333" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13904,7 +13913,7 @@
       <c r="E334" s="3"/>
       <c r="G334" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H334" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13924,7 +13933,7 @@
       <c r="E335" s="3"/>
       <c r="G335" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H335" s="16" t="str">
         <f t="shared" si="10"/>
@@ -13944,7 +13953,7 @@
       <c r="E336" s="3"/>
       <c r="G336" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H336" s="16" t="str">
         <f t="shared" ref="H336:H399" si="12">IF(EXACT(D336, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B336, ""), "null", B336), "::bigint, ", IF(EXACT(D336, ""), "null", D336), "::bigint, ", IF(EXACT(E336, ""), "null", E336), "::bigint);"))</f>
@@ -13964,7 +13973,7 @@
       <c r="E337" s="3"/>
       <c r="G337" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H337" s="16" t="str">
         <f t="shared" si="12"/>
@@ -13984,7 +13993,7 @@
       <c r="E338" s="3"/>
       <c r="G338" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H338" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14004,7 +14013,7 @@
       <c r="E339" s="3"/>
       <c r="G339" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H339" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14024,7 +14033,7 @@
       <c r="E340" s="3"/>
       <c r="G340" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H340" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14044,7 +14053,7 @@
       <c r="E341" s="3"/>
       <c r="G341" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H341" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14064,7 +14073,7 @@
       <c r="E342" s="3"/>
       <c r="G342" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H342" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14084,7 +14093,7 @@
       <c r="E343" s="3"/>
       <c r="G343" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H343" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14104,7 +14113,7 @@
       <c r="E344" s="3"/>
       <c r="G344" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H344" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14124,7 +14133,7 @@
       <c r="E345" s="3"/>
       <c r="G345" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H345" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14144,7 +14153,7 @@
       <c r="E346" s="3"/>
       <c r="G346" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H346" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14164,7 +14173,7 @@
       <c r="E347" s="3"/>
       <c r="G347" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H347" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14184,7 +14193,7 @@
       <c r="E348" s="3"/>
       <c r="G348" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H348" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14204,7 +14213,7 @@
       <c r="E349" s="3"/>
       <c r="G349" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="H349" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14226,7 +14235,7 @@
       <c r="E350" s="3"/>
       <c r="G350" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H350" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14246,7 +14255,7 @@
       <c r="E351" s="3"/>
       <c r="G351" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H351" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14266,7 +14275,7 @@
       <c r="E352" s="3"/>
       <c r="G352" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H352" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14286,7 +14295,7 @@
       <c r="E353" s="3"/>
       <c r="G353" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H353" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14306,7 +14315,7 @@
       <c r="E354" s="3"/>
       <c r="G354" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H354" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14326,7 +14335,7 @@
       <c r="E355" s="3"/>
       <c r="G355" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H355" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14346,7 +14355,7 @@
       <c r="E356" s="3"/>
       <c r="G356" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H356" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14366,7 +14375,7 @@
       <c r="E357" s="3"/>
       <c r="G357" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H357" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14386,7 +14395,7 @@
       <c r="E358" s="3"/>
       <c r="G358" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H358" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14406,7 +14415,7 @@
       <c r="E359" s="3"/>
       <c r="G359" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H359" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14426,7 +14435,7 @@
       <c r="E360" s="3"/>
       <c r="G360" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H360" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14446,7 +14455,7 @@
       <c r="E361" s="3"/>
       <c r="G361" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H361" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14466,7 +14475,7 @@
       <c r="E362" s="3"/>
       <c r="G362" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H362" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14486,7 +14495,7 @@
       <c r="E363" s="3"/>
       <c r="G363" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H363" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14506,7 +14515,7 @@
       <c r="E364" s="3"/>
       <c r="G364" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H364" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14526,7 +14535,7 @@
       <c r="E365" s="3"/>
       <c r="G365" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H365" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14546,7 +14555,7 @@
       <c r="E366" s="3"/>
       <c r="G366" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H366" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14566,7 +14575,7 @@
       <c r="E367" s="3"/>
       <c r="G367" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H367" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14586,7 +14595,7 @@
       <c r="E368" s="3"/>
       <c r="G368" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H368" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14606,7 +14615,7 @@
       <c r="E369" s="3"/>
       <c r="G369" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H369" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14626,7 +14635,7 @@
       <c r="E370" s="3"/>
       <c r="G370" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H370" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14646,7 +14655,7 @@
       <c r="E371" s="3"/>
       <c r="G371" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H371" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14666,7 +14675,7 @@
       <c r="E372" s="3"/>
       <c r="G372" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H372" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14686,7 +14695,7 @@
       <c r="E373" s="3"/>
       <c r="G373" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H373" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14706,7 +14715,7 @@
       <c r="E374" s="3"/>
       <c r="G374" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H374" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14726,7 +14735,7 @@
       <c r="E375" s="3"/>
       <c r="G375" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H375" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14746,7 +14755,7 @@
       <c r="E376" s="3"/>
       <c r="G376" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H376" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14766,7 +14775,7 @@
       <c r="E377" s="3"/>
       <c r="G377" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H377" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14786,7 +14795,7 @@
       <c r="E378" s="3"/>
       <c r="G378" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H378" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14806,7 +14815,7 @@
       <c r="E379" s="3"/>
       <c r="G379" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H379" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14826,7 +14835,7 @@
       <c r="E380" s="3"/>
       <c r="G380" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H380" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14846,7 +14855,7 @@
       <c r="E381" s="3"/>
       <c r="G381" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H381" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14866,7 +14875,7 @@
       <c r="E382" s="3"/>
       <c r="G382" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H382" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14886,7 +14895,7 @@
       <c r="E383" s="3"/>
       <c r="G383" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H383" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14906,7 +14915,7 @@
       <c r="E384" s="3"/>
       <c r="G384" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H384" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14926,7 +14935,7 @@
       <c r="E385" s="3"/>
       <c r="G385" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H385" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14946,7 +14955,7 @@
       <c r="E386" s="3"/>
       <c r="G386" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H386" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14966,7 +14975,7 @@
       <c r="E387" s="3"/>
       <c r="G387" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H387" s="16" t="str">
         <f t="shared" si="12"/>
@@ -14986,7 +14995,7 @@
       <c r="E388" s="3"/>
       <c r="G388" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H388" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15006,7 +15015,7 @@
       <c r="E389" s="3"/>
       <c r="G389" s="15">
         <f t="shared" si="11"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H389" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15026,7 +15035,7 @@
       <c r="E390" s="3"/>
       <c r="G390" s="15">
         <f t="shared" ref="G390:G453" si="13" xml:space="preserve"> G389 + IF(EXACT(H390, ""), 0, 1)</f>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H390" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15046,7 +15055,7 @@
       <c r="E391" s="3"/>
       <c r="G391" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H391" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15066,7 +15075,7 @@
       <c r="E392" s="3"/>
       <c r="G392" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H392" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15086,7 +15095,7 @@
       <c r="E393" s="3"/>
       <c r="G393" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="H393" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15108,7 +15117,7 @@
       <c r="E394" s="3"/>
       <c r="G394" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="H394" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15128,7 +15137,7 @@
       <c r="E395" s="3"/>
       <c r="G395" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="H395" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15148,7 +15157,7 @@
       <c r="E396" s="3"/>
       <c r="G396" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="H396" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15168,7 +15177,7 @@
       <c r="E397" s="3"/>
       <c r="G397" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="H397" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15188,7 +15197,7 @@
       <c r="E398" s="3"/>
       <c r="G398" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="H398" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15208,7 +15217,7 @@
       <c r="E399" s="3"/>
       <c r="G399" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="H399" s="16" t="str">
         <f t="shared" si="12"/>
@@ -15230,7 +15239,7 @@
       <c r="E400" s="3"/>
       <c r="G400" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H400" s="16" t="str">
         <f t="shared" ref="H400:H463" si="14">IF(EXACT(D400, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B400, ""), "null", B400), "::bigint, ", IF(EXACT(D400, ""), "null", D400), "::bigint, ", IF(EXACT(E400, ""), "null", E400), "::bigint);"))</f>
@@ -15250,7 +15259,7 @@
       <c r="E401" s="3"/>
       <c r="G401" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H401" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15270,7 +15279,7 @@
       <c r="E402" s="3"/>
       <c r="G402" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H402" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15290,7 +15299,7 @@
       <c r="E403" s="3"/>
       <c r="G403" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H403" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15310,7 +15319,7 @@
       <c r="E404" s="3"/>
       <c r="G404" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H404" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15330,7 +15339,7 @@
       <c r="E405" s="3"/>
       <c r="G405" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H405" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15350,7 +15359,7 @@
       <c r="E406" s="3"/>
       <c r="G406" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H406" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15370,7 +15379,7 @@
       <c r="E407" s="3"/>
       <c r="G407" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H407" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15390,7 +15399,7 @@
       <c r="E408" s="3"/>
       <c r="G408" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H408" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15410,7 +15419,7 @@
       <c r="E409" s="3"/>
       <c r="G409" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H409" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15430,7 +15439,7 @@
       <c r="E410" s="3"/>
       <c r="G410" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H410" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15450,7 +15459,7 @@
       <c r="E411" s="3"/>
       <c r="G411" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H411" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15470,7 +15479,7 @@
       <c r="E412" s="3"/>
       <c r="G412" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H412" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15490,7 +15499,7 @@
       <c r="E413" s="3"/>
       <c r="G413" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H413" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15510,7 +15519,7 @@
       <c r="E414" s="3"/>
       <c r="G414" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H414" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15530,7 +15539,7 @@
       <c r="E415" s="3"/>
       <c r="G415" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="H415" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15552,7 +15561,7 @@
       <c r="E416" s="3"/>
       <c r="G416" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H416" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15572,7 +15581,7 @@
       <c r="E417" s="3"/>
       <c r="G417" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H417" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15592,7 +15601,7 @@
       <c r="E418" s="3"/>
       <c r="G418" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H418" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15612,7 +15621,7 @@
       <c r="E419" s="3"/>
       <c r="G419" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H419" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15632,7 +15641,7 @@
       <c r="E420" s="3"/>
       <c r="G420" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H420" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15652,7 +15661,7 @@
       <c r="E421" s="3"/>
       <c r="G421" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H421" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15672,7 +15681,7 @@
       <c r="E422" s="3"/>
       <c r="G422" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H422" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15692,7 +15701,7 @@
       <c r="E423" s="3"/>
       <c r="G423" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H423" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15712,7 +15721,7 @@
       <c r="E424" s="3"/>
       <c r="G424" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H424" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15732,7 +15741,7 @@
       <c r="E425" s="3"/>
       <c r="G425" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H425" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15752,7 +15761,7 @@
       <c r="E426" s="3"/>
       <c r="G426" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H426" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15772,7 +15781,7 @@
       <c r="E427" s="3"/>
       <c r="G427" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H427" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15792,7 +15801,7 @@
       <c r="E428" s="3"/>
       <c r="G428" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H428" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15812,7 +15821,7 @@
       <c r="E429" s="3"/>
       <c r="G429" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H429" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15832,7 +15841,7 @@
       <c r="E430" s="3"/>
       <c r="G430" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="H430" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15854,7 +15863,7 @@
       <c r="E431" s="3"/>
       <c r="G431" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H431" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15874,7 +15883,7 @@
       <c r="E432" s="3"/>
       <c r="G432" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H432" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15894,7 +15903,7 @@
       <c r="E433" s="3"/>
       <c r="G433" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H433" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15914,7 +15923,7 @@
       <c r="E434" s="3"/>
       <c r="G434" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H434" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15934,7 +15943,7 @@
       <c r="E435" s="3"/>
       <c r="G435" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H435" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15954,7 +15963,7 @@
       <c r="E436" s="3"/>
       <c r="G436" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H436" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15974,7 +15983,7 @@
       <c r="E437" s="3"/>
       <c r="G437" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H437" s="16" t="str">
         <f t="shared" si="14"/>
@@ -15994,7 +16003,7 @@
       <c r="E438" s="3"/>
       <c r="G438" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H438" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16014,7 +16023,7 @@
       <c r="E439" s="3"/>
       <c r="G439" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H439" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16034,7 +16043,7 @@
       <c r="E440" s="3"/>
       <c r="G440" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H440" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16054,7 +16063,7 @@
       <c r="E441" s="3"/>
       <c r="G441" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="H441" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16076,7 +16085,7 @@
       <c r="E442" s="3"/>
       <c r="G442" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H442" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16096,7 +16105,7 @@
       <c r="E443" s="3"/>
       <c r="G443" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H443" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16116,7 +16125,7 @@
       <c r="E444" s="3"/>
       <c r="G444" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H444" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16136,7 +16145,7 @@
       <c r="E445" s="3"/>
       <c r="G445" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H445" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16156,7 +16165,7 @@
       <c r="E446" s="3"/>
       <c r="G446" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H446" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16176,7 +16185,7 @@
       <c r="E447" s="3"/>
       <c r="G447" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H447" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16196,7 +16205,7 @@
       <c r="E448" s="3"/>
       <c r="G448" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H448" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16216,7 +16225,7 @@
       <c r="E449" s="3"/>
       <c r="G449" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H449" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16236,7 +16245,7 @@
       <c r="E450" s="3"/>
       <c r="G450" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H450" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16256,7 +16265,7 @@
       <c r="E451" s="3"/>
       <c r="G451" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H451" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16276,7 +16285,7 @@
       <c r="E452" s="3"/>
       <c r="G452" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H452" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16296,7 +16305,7 @@
       <c r="E453" s="3"/>
       <c r="G453" s="15">
         <f t="shared" si="13"/>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H453" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16316,7 +16325,7 @@
       <c r="E454" s="3"/>
       <c r="G454" s="15">
         <f t="shared" ref="G454:G517" si="15" xml:space="preserve"> G453 + IF(EXACT(H454, ""), 0, 1)</f>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="H454" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16338,7 +16347,7 @@
       <c r="E455" s="3"/>
       <c r="G455" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H455" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16358,7 +16367,7 @@
       <c r="E456" s="3"/>
       <c r="G456" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H456" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16378,7 +16387,7 @@
       <c r="E457" s="3"/>
       <c r="G457" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H457" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16398,7 +16407,7 @@
       <c r="E458" s="3"/>
       <c r="G458" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H458" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16418,7 +16427,7 @@
       <c r="E459" s="3"/>
       <c r="G459" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H459" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16438,7 +16447,7 @@
       <c r="E460" s="3"/>
       <c r="G460" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H460" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16458,7 +16467,7 @@
       <c r="E461" s="3"/>
       <c r="G461" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H461" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16478,7 +16487,7 @@
       <c r="E462" s="3"/>
       <c r="G462" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H462" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16498,7 +16507,7 @@
       <c r="E463" s="3"/>
       <c r="G463" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H463" s="16" t="str">
         <f t="shared" si="14"/>
@@ -16518,7 +16527,7 @@
       <c r="E464" s="3"/>
       <c r="G464" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H464" s="16" t="str">
         <f t="shared" ref="H464:H527" si="16">IF(EXACT(D464, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B464, ""), "null", B464), "::bigint, ", IF(EXACT(D464, ""), "null", D464), "::bigint, ", IF(EXACT(E464, ""), "null", E464), "::bigint);"))</f>
@@ -16538,7 +16547,7 @@
       <c r="E465" s="3"/>
       <c r="G465" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H465" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16558,7 +16567,7 @@
       <c r="E466" s="3"/>
       <c r="G466" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H466" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16578,7 +16587,7 @@
       <c r="E467" s="3"/>
       <c r="G467" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H467" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16598,7 +16607,7 @@
       <c r="E468" s="3"/>
       <c r="G468" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H468" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16618,7 +16627,7 @@
       <c r="E469" s="3"/>
       <c r="G469" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H469" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16638,7 +16647,7 @@
       <c r="E470" s="3"/>
       <c r="G470" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H470" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16658,7 +16667,7 @@
       <c r="E471" s="3"/>
       <c r="G471" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H471" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16678,7 +16687,7 @@
       <c r="E472" s="3"/>
       <c r="G472" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H472" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16698,7 +16707,7 @@
       <c r="E473" s="3"/>
       <c r="G473" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H473" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16718,7 +16727,7 @@
       <c r="E474" s="3"/>
       <c r="G474" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H474" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16738,7 +16747,7 @@
       <c r="E475" s="3"/>
       <c r="G475" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H475" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16758,7 +16767,7 @@
       <c r="E476" s="3"/>
       <c r="G476" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H476" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16778,7 +16787,7 @@
       <c r="E477" s="3"/>
       <c r="G477" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H477" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16798,7 +16807,7 @@
       <c r="E478" s="3"/>
       <c r="G478" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H478" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16818,7 +16827,7 @@
       <c r="E479" s="3"/>
       <c r="G479" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H479" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16838,7 +16847,7 @@
       <c r="E480" s="3"/>
       <c r="G480" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H480" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16858,7 +16867,7 @@
       <c r="E481" s="3"/>
       <c r="G481" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H481" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16878,7 +16887,7 @@
       <c r="E482" s="3"/>
       <c r="G482" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H482" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16898,7 +16907,7 @@
       <c r="E483" s="3"/>
       <c r="G483" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H483" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16918,7 +16927,7 @@
       <c r="E484" s="3"/>
       <c r="G484" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H484" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16938,7 +16947,7 @@
       <c r="E485" s="3"/>
       <c r="G485" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H485" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16958,7 +16967,7 @@
       <c r="E486" s="3"/>
       <c r="G486" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H486" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16978,7 +16987,7 @@
       <c r="E487" s="3"/>
       <c r="G487" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H487" s="16" t="str">
         <f t="shared" si="16"/>
@@ -16998,7 +17007,7 @@
       <c r="E488" s="3"/>
       <c r="G488" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H488" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17018,7 +17027,7 @@
       <c r="E489" s="3"/>
       <c r="G489" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="H489" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17040,7 +17049,7 @@
       <c r="E490" s="3"/>
       <c r="G490" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H490" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17060,7 +17069,7 @@
       <c r="E491" s="3"/>
       <c r="G491" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H491" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17080,7 +17089,7 @@
       <c r="E492" s="3"/>
       <c r="G492" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H492" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17100,7 +17109,7 @@
       <c r="E493" s="3"/>
       <c r="G493" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H493" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17120,7 +17129,7 @@
       <c r="E494" s="3"/>
       <c r="G494" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H494" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17140,7 +17149,7 @@
       <c r="E495" s="3"/>
       <c r="G495" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H495" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17160,7 +17169,7 @@
       <c r="E496" s="3"/>
       <c r="G496" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H496" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17180,7 +17189,7 @@
       <c r="E497" s="3"/>
       <c r="G497" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H497" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17200,7 +17209,7 @@
       <c r="E498" s="3"/>
       <c r="G498" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H498" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17220,7 +17229,7 @@
       <c r="E499" s="3"/>
       <c r="G499" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="H499" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17242,7 +17251,7 @@
       <c r="E500" s="3"/>
       <c r="G500" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H500" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17262,7 +17271,7 @@
       <c r="E501" s="3"/>
       <c r="G501" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H501" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17282,7 +17291,7 @@
       <c r="E502" s="3"/>
       <c r="G502" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H502" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17302,7 +17311,7 @@
       <c r="E503" s="3"/>
       <c r="G503" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H503" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17322,7 +17331,7 @@
       <c r="E504" s="3"/>
       <c r="G504" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H504" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17342,7 +17351,7 @@
       <c r="E505" s="3"/>
       <c r="G505" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H505" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17362,7 +17371,7 @@
       <c r="E506" s="3"/>
       <c r="G506" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H506" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17382,7 +17391,7 @@
       <c r="E507" s="3"/>
       <c r="G507" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H507" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17402,7 +17411,7 @@
       <c r="E508" s="3"/>
       <c r="G508" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H508" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17422,7 +17431,7 @@
       <c r="E509" s="3"/>
       <c r="G509" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H509" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17442,7 +17451,7 @@
       <c r="E510" s="3"/>
       <c r="G510" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H510" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17462,7 +17471,7 @@
       <c r="E511" s="3"/>
       <c r="G511" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H511" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17482,7 +17491,7 @@
       <c r="E512" s="3"/>
       <c r="G512" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H512" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17502,7 +17511,7 @@
       <c r="E513" s="3"/>
       <c r="G513" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H513" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17522,7 +17531,7 @@
       <c r="E514" s="3"/>
       <c r="G514" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H514" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17542,7 +17551,7 @@
       <c r="E515" s="3"/>
       <c r="G515" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H515" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17562,7 +17571,7 @@
       <c r="E516" s="3"/>
       <c r="G516" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H516" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17582,7 +17591,7 @@
       <c r="E517" s="3"/>
       <c r="G517" s="15">
         <f t="shared" si="15"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H517" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17602,7 +17611,7 @@
       <c r="E518" s="3"/>
       <c r="G518" s="15">
         <f t="shared" ref="G518:G581" si="17" xml:space="preserve"> G517 + IF(EXACT(H518, ""), 0, 1)</f>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H518" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17622,7 +17631,7 @@
       <c r="E519" s="3"/>
       <c r="G519" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H519" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17642,7 +17651,7 @@
       <c r="E520" s="3"/>
       <c r="G520" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H520" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17662,7 +17671,7 @@
       <c r="E521" s="3"/>
       <c r="G521" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H521" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17682,7 +17691,7 @@
       <c r="E522" s="3"/>
       <c r="G522" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H522" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17702,7 +17711,7 @@
       <c r="E523" s="3"/>
       <c r="G523" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H523" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17722,7 +17731,7 @@
       <c r="E524" s="3"/>
       <c r="G524" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="H524" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17744,7 +17753,7 @@
       <c r="E525" s="3"/>
       <c r="G525" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000027</v>
+        <v>225000000000028</v>
       </c>
       <c r="H525" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17764,7 +17773,7 @@
       <c r="E526" s="3"/>
       <c r="G526" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000027</v>
+        <v>225000000000028</v>
       </c>
       <c r="H526" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17784,7 +17793,7 @@
       <c r="E527" s="3"/>
       <c r="G527" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000027</v>
+        <v>225000000000028</v>
       </c>
       <c r="H527" s="16" t="str">
         <f t="shared" si="16"/>
@@ -17804,7 +17813,7 @@
       <c r="E528" s="3"/>
       <c r="G528" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000027</v>
+        <v>225000000000028</v>
       </c>
       <c r="H528" s="16" t="str">
         <f t="shared" ref="H528:H589" si="18">IF(EXACT(D528, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B528, ""), "null", B528), "::bigint, ", IF(EXACT(D528, ""), "null", D528), "::bigint, ", IF(EXACT(E528, ""), "null", E528), "::bigint);"))</f>
@@ -17824,7 +17833,7 @@
       <c r="E529" s="3"/>
       <c r="G529" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000027</v>
+        <v>225000000000028</v>
       </c>
       <c r="H529" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17846,7 +17855,7 @@
       <c r="E530" s="3"/>
       <c r="G530" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H530" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17866,7 +17875,7 @@
       <c r="E531" s="3"/>
       <c r="G531" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H531" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17886,7 +17895,7 @@
       <c r="E532" s="3"/>
       <c r="G532" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H532" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17906,7 +17915,7 @@
       <c r="E533" s="3"/>
       <c r="G533" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H533" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17926,7 +17935,7 @@
       <c r="E534" s="3"/>
       <c r="G534" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H534" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17946,7 +17955,7 @@
       <c r="E535" s="3"/>
       <c r="G535" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H535" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17966,7 +17975,7 @@
       <c r="E536" s="3"/>
       <c r="G536" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H536" s="16" t="str">
         <f t="shared" si="18"/>
@@ -17986,7 +17995,7 @@
       <c r="E537" s="3"/>
       <c r="G537" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H537" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18006,7 +18015,7 @@
       <c r="E538" s="3"/>
       <c r="G538" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="H538" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18028,7 +18037,7 @@
       <c r="E539" s="3"/>
       <c r="G539" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="H539" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18048,7 +18057,7 @@
       <c r="E540" s="3"/>
       <c r="G540" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="H540" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18068,7 +18077,7 @@
       <c r="E541" s="3"/>
       <c r="G541" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="H541" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18088,7 +18097,7 @@
       <c r="E542" s="3"/>
       <c r="G542" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="H542" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18108,7 +18117,7 @@
       <c r="E543" s="3"/>
       <c r="G543" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="H543" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18128,7 +18137,7 @@
       <c r="E544" s="3"/>
       <c r="G544" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="H544" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18147,14 +18156,16 @@
       <c r="D545" s="3">
         <v>95000000000023</v>
       </c>
-      <c r="E545" s="3"/>
+      <c r="E545" s="3">
+        <v>46000000000033</v>
+      </c>
       <c r="G545" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000030</v>
+        <v>225000000000031</v>
       </c>
       <c r="H545" s="16" t="str">
         <f t="shared" si="18"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000542::bigint, 95000000000023::bigint, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000542::bigint, 95000000000023::bigint, 46000000000033::bigint);</v>
       </c>
     </row>
     <row r="546" spans="2:8" x14ac:dyDescent="0.2">
@@ -18170,7 +18181,7 @@
       <c r="E546" s="3"/>
       <c r="G546" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000030</v>
+        <v>225000000000031</v>
       </c>
       <c r="H546" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18190,7 +18201,7 @@
       <c r="E547" s="3"/>
       <c r="G547" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000030</v>
+        <v>225000000000031</v>
       </c>
       <c r="H547" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18212,7 +18223,7 @@
       <c r="E548" s="3"/>
       <c r="G548" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000031</v>
+        <v>225000000000032</v>
       </c>
       <c r="H548" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18232,7 +18243,7 @@
       <c r="E549" s="3"/>
       <c r="G549" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000031</v>
+        <v>225000000000032</v>
       </c>
       <c r="H549" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18254,7 +18265,7 @@
       <c r="E550" s="3"/>
       <c r="G550" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H550" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18274,7 +18285,7 @@
       <c r="E551" s="3"/>
       <c r="G551" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H551" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18294,7 +18305,7 @@
       <c r="E552" s="3"/>
       <c r="G552" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H552" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18314,7 +18325,7 @@
       <c r="E553" s="3"/>
       <c r="G553" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H553" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18334,7 +18345,7 @@
       <c r="E554" s="3"/>
       <c r="G554" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H554" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18354,7 +18365,7 @@
       <c r="E555" s="3"/>
       <c r="G555" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H555" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18374,7 +18385,7 @@
       <c r="E556" s="3"/>
       <c r="G556" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H556" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18394,7 +18405,7 @@
       <c r="E557" s="3"/>
       <c r="G557" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H557" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18414,7 +18425,7 @@
       <c r="E558" s="3"/>
       <c r="G558" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H558" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18434,7 +18445,7 @@
       <c r="E559" s="3"/>
       <c r="G559" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H559" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18454,7 +18465,7 @@
       <c r="E560" s="3"/>
       <c r="G560" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H560" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18474,7 +18485,7 @@
       <c r="E561" s="3"/>
       <c r="G561" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="H561" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18490,15 +18501,17 @@
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M562, ""), "", '[1]Internal Career (Last Position)'!$C562)</f>
         <v>Adhe Kurniawan</v>
       </c>
-      <c r="D562" s="3"/>
+      <c r="D562" s="3">
+        <v>95000000000015</v>
+      </c>
       <c r="E562" s="3"/>
       <c r="G562" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H562" s="16" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000559::bigint, 95000000000015::bigint, null::bigint);</v>
       </c>
     </row>
     <row r="563" spans="2:8" x14ac:dyDescent="0.2">
@@ -18514,7 +18527,7 @@
       <c r="E563" s="3"/>
       <c r="G563" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H563" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18534,7 +18547,7 @@
       <c r="E564" s="3"/>
       <c r="G564" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H564" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18554,7 +18567,7 @@
       <c r="E565" s="3"/>
       <c r="G565" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H565" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18574,7 +18587,7 @@
       <c r="E566" s="3"/>
       <c r="G566" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H566" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18594,7 +18607,7 @@
       <c r="E567" s="3"/>
       <c r="G567" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H567" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18614,7 +18627,7 @@
       <c r="E568" s="3"/>
       <c r="G568" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H568" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18634,7 +18647,7 @@
       <c r="E569" s="3"/>
       <c r="G569" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H569" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18654,7 +18667,7 @@
       <c r="E570" s="3"/>
       <c r="G570" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H570" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18674,7 +18687,7 @@
       <c r="E571" s="3"/>
       <c r="G571" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H571" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18694,7 +18707,7 @@
       <c r="E572" s="3"/>
       <c r="G572" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H572" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18714,7 +18727,7 @@
       <c r="E573" s="3"/>
       <c r="G573" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H573" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18734,7 +18747,7 @@
       <c r="E574" s="3"/>
       <c r="G574" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H574" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18754,7 +18767,7 @@
       <c r="E575" s="3"/>
       <c r="G575" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H575" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18774,7 +18787,7 @@
       <c r="E576" s="3"/>
       <c r="G576" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H576" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18794,7 +18807,7 @@
       <c r="E577" s="3"/>
       <c r="G577" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H577" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18814,7 +18827,7 @@
       <c r="E578" s="3"/>
       <c r="G578" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H578" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18834,7 +18847,7 @@
       <c r="E579" s="3"/>
       <c r="G579" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H579" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18854,7 +18867,7 @@
       <c r="E580" s="3"/>
       <c r="G580" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H580" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18874,7 +18887,7 @@
       <c r="E581" s="3"/>
       <c r="G581" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H581" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18894,7 +18907,7 @@
       <c r="E582" s="3"/>
       <c r="G582" s="15">
         <f t="shared" ref="G582:G589" si="19" xml:space="preserve"> G581 + IF(EXACT(H582, ""), 0, 1)</f>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H582" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18914,7 +18927,7 @@
       <c r="E583" s="3"/>
       <c r="G583" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H583" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18934,7 +18947,7 @@
       <c r="E584" s="3"/>
       <c r="G584" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000032</v>
+        <v>225000000000034</v>
       </c>
       <c r="H584" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18956,7 +18969,7 @@
       <c r="E585" s="3"/>
       <c r="G585" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000033</v>
+        <v>225000000000035</v>
       </c>
       <c r="H585" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18976,7 +18989,7 @@
       <c r="E586" s="3"/>
       <c r="G586" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000033</v>
+        <v>225000000000035</v>
       </c>
       <c r="H586" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18996,7 +19009,7 @@
       <c r="E587" s="3"/>
       <c r="G587" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000033</v>
+        <v>225000000000035</v>
       </c>
       <c r="H587" s="16" t="str">
         <f t="shared" si="18"/>
@@ -19016,7 +19029,7 @@
       <c r="E588" s="3"/>
       <c r="G588" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000033</v>
+        <v>225000000000035</v>
       </c>
       <c r="H588" s="16" t="str">
         <f t="shared" si="18"/>
@@ -19036,7 +19049,7 @@
       <c r="E589" s="4"/>
       <c r="G589" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000033</v>
+        <v>225000000000035</v>
       </c>
       <c r="H589" s="17" t="str">
         <f t="shared" si="18"/>
@@ -21891,7 +21904,7 @@
       </c>
       <c r="F128" s="28" t="str">
         <f>IF(EXACT(MAIN!$H128, ""), "", ""&amp;MAIN!$E128)</f>
-        <v/>
+        <v>46000000000009</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.2">
@@ -22511,21 +22524,21 @@
       </c>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B157" s="26">
+      <c r="B157" s="26" t="str">
         <f>IF(EXACT(MAIN!H157, ""), "", MAIN!G157)</f>
-        <v>225000000000009</v>
-      </c>
-      <c r="C157" s="3">
+        <v/>
+      </c>
+      <c r="C157" s="3" t="str">
         <f>IF(EXACT(MAIN!$H157, ""), "", MAIN!$B157)</f>
-        <v>164000000000154</v>
+        <v/>
       </c>
       <c r="D157" s="3" t="str">
         <f>IF(EXACT(MAIN!$H157, ""), "", MAIN!$C157)</f>
-        <v>Fikri</v>
-      </c>
-      <c r="E157" s="3">
+        <v/>
+      </c>
+      <c r="E157" s="3" t="str">
         <f>IF(EXACT(MAIN!$H157, ""), "", MAIN!$D157)</f>
-        <v>95000000000023</v>
+        <v/>
       </c>
       <c r="F157" s="28" t="str">
         <f>IF(EXACT(MAIN!$H157, ""), "", ""&amp;MAIN!$E157)</f>
@@ -22533,25 +22546,25 @@
       </c>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B158" s="26" t="str">
+      <c r="B158" s="26">
         <f>IF(EXACT(MAIN!H158, ""), "", MAIN!G158)</f>
-        <v/>
-      </c>
-      <c r="C158" s="3" t="str">
+        <v>225000000000009</v>
+      </c>
+      <c r="C158" s="3">
         <f>IF(EXACT(MAIN!$H158, ""), "", MAIN!$B158)</f>
-        <v/>
+        <v>164000000000155</v>
       </c>
       <c r="D158" s="3" t="str">
         <f>IF(EXACT(MAIN!$H158, ""), "", MAIN!$C158)</f>
-        <v/>
-      </c>
-      <c r="E158" s="3" t="str">
+        <v>M. Fikri Caesarandi Hasibuan</v>
+      </c>
+      <c r="E158" s="3">
         <f>IF(EXACT(MAIN!$H158, ""), "", MAIN!$D158)</f>
-        <v/>
+        <v>95000000000023</v>
       </c>
       <c r="F158" s="28" t="str">
         <f>IF(EXACT(MAIN!$H158, ""), "", ""&amp;MAIN!$E158)</f>
-        <v/>
+        <v>46000000000033</v>
       </c>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.2">
@@ -24245,7 +24258,7 @@
       </c>
       <c r="F235" s="28" t="str">
         <f>IF(EXACT(MAIN!$H235, ""), "", ""&amp;MAIN!$E235)</f>
-        <v/>
+        <v>46000000000033</v>
       </c>
     </row>
     <row r="236" spans="2:6" x14ac:dyDescent="0.2">
@@ -25239,25 +25252,25 @@
       </c>
     </row>
     <row r="281" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B281" s="26" t="str">
+      <c r="B281" s="26">
         <f>IF(EXACT(MAIN!H281, ""), "", MAIN!G281)</f>
-        <v/>
-      </c>
-      <c r="C281" s="3" t="str">
+        <v>225000000000017</v>
+      </c>
+      <c r="C281" s="3">
         <f>IF(EXACT(MAIN!$H281, ""), "", MAIN!$B281)</f>
-        <v/>
+        <v>164000000000278</v>
       </c>
       <c r="D281" s="3" t="str">
         <f>IF(EXACT(MAIN!$H281, ""), "", MAIN!$C281)</f>
-        <v/>
-      </c>
-      <c r="E281" s="3" t="str">
+        <v>T. Marungkil U. S. Sagala</v>
+      </c>
+      <c r="E281" s="3">
         <f>IF(EXACT(MAIN!$H281, ""), "", MAIN!$D281)</f>
-        <v/>
+        <v>95000000000018</v>
       </c>
       <c r="F281" s="28" t="str">
         <f>IF(EXACT(MAIN!$H281, ""), "", ""&amp;MAIN!$E281)</f>
-        <v/>
+        <v>46000000000009</v>
       </c>
     </row>
     <row r="282" spans="2:6" x14ac:dyDescent="0.2">
@@ -25747,7 +25760,7 @@
     <row r="304" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B304" s="26">
         <f>IF(EXACT(MAIN!H304, ""), "", MAIN!G304)</f>
-        <v>225000000000017</v>
+        <v>225000000000018</v>
       </c>
       <c r="C304" s="3">
         <f>IF(EXACT(MAIN!$H304, ""), "", MAIN!$B304)</f>
@@ -26759,7 +26772,7 @@
     <row r="350" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B350" s="26">
         <f>IF(EXACT(MAIN!H350, ""), "", MAIN!G350)</f>
-        <v>225000000000018</v>
+        <v>225000000000019</v>
       </c>
       <c r="C350" s="3">
         <f>IF(EXACT(MAIN!$H350, ""), "", MAIN!$B350)</f>
@@ -27727,7 +27740,7 @@
     <row r="394" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B394" s="26">
         <f>IF(EXACT(MAIN!H394, ""), "", MAIN!G394)</f>
-        <v>225000000000019</v>
+        <v>225000000000020</v>
       </c>
       <c r="C394" s="3">
         <f>IF(EXACT(MAIN!$H394, ""), "", MAIN!$B394)</f>
@@ -27859,7 +27872,7 @@
     <row r="400" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B400" s="26">
         <f>IF(EXACT(MAIN!H400, ""), "", MAIN!G400)</f>
-        <v>225000000000020</v>
+        <v>225000000000021</v>
       </c>
       <c r="C400" s="3">
         <f>IF(EXACT(MAIN!$H400, ""), "", MAIN!$B400)</f>
@@ -28211,7 +28224,7 @@
     <row r="416" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B416" s="26">
         <f>IF(EXACT(MAIN!H416, ""), "", MAIN!G416)</f>
-        <v>225000000000021</v>
+        <v>225000000000022</v>
       </c>
       <c r="C416" s="3">
         <f>IF(EXACT(MAIN!$H416, ""), "", MAIN!$B416)</f>
@@ -28541,7 +28554,7 @@
     <row r="431" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B431" s="26">
         <f>IF(EXACT(MAIN!H431, ""), "", MAIN!G431)</f>
-        <v>225000000000022</v>
+        <v>225000000000023</v>
       </c>
       <c r="C431" s="3">
         <f>IF(EXACT(MAIN!$H431, ""), "", MAIN!$B431)</f>
@@ -28783,7 +28796,7 @@
     <row r="442" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B442" s="26">
         <f>IF(EXACT(MAIN!H442, ""), "", MAIN!G442)</f>
-        <v>225000000000023</v>
+        <v>225000000000024</v>
       </c>
       <c r="C442" s="3">
         <f>IF(EXACT(MAIN!$H442, ""), "", MAIN!$B442)</f>
@@ -29069,7 +29082,7 @@
     <row r="455" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B455" s="26">
         <f>IF(EXACT(MAIN!H455, ""), "", MAIN!G455)</f>
-        <v>225000000000024</v>
+        <v>225000000000025</v>
       </c>
       <c r="C455" s="3">
         <f>IF(EXACT(MAIN!$H455, ""), "", MAIN!$B455)</f>
@@ -29839,7 +29852,7 @@
     <row r="490" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B490" s="26">
         <f>IF(EXACT(MAIN!H490, ""), "", MAIN!G490)</f>
-        <v>225000000000025</v>
+        <v>225000000000026</v>
       </c>
       <c r="C490" s="3">
         <f>IF(EXACT(MAIN!$H490, ""), "", MAIN!$B490)</f>
@@ -30059,7 +30072,7 @@
     <row r="500" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B500" s="26">
         <f>IF(EXACT(MAIN!H500, ""), "", MAIN!G500)</f>
-        <v>225000000000026</v>
+        <v>225000000000027</v>
       </c>
       <c r="C500" s="3">
         <f>IF(EXACT(MAIN!$H500, ""), "", MAIN!$B500)</f>
@@ -30609,7 +30622,7 @@
     <row r="525" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B525" s="26">
         <f>IF(EXACT(MAIN!H525, ""), "", MAIN!G525)</f>
-        <v>225000000000027</v>
+        <v>225000000000028</v>
       </c>
       <c r="C525" s="3">
         <f>IF(EXACT(MAIN!$H525, ""), "", MAIN!$B525)</f>
@@ -30719,7 +30732,7 @@
     <row r="530" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B530" s="26">
         <f>IF(EXACT(MAIN!H530, ""), "", MAIN!G530)</f>
-        <v>225000000000028</v>
+        <v>225000000000029</v>
       </c>
       <c r="C530" s="3">
         <f>IF(EXACT(MAIN!$H530, ""), "", MAIN!$B530)</f>
@@ -30917,7 +30930,7 @@
     <row r="539" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B539" s="26">
         <f>IF(EXACT(MAIN!H539, ""), "", MAIN!G539)</f>
-        <v>225000000000029</v>
+        <v>225000000000030</v>
       </c>
       <c r="C539" s="3">
         <f>IF(EXACT(MAIN!$H539, ""), "", MAIN!$B539)</f>
@@ -31049,7 +31062,7 @@
     <row r="545" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B545" s="26">
         <f>IF(EXACT(MAIN!H545, ""), "", MAIN!G545)</f>
-        <v>225000000000030</v>
+        <v>225000000000031</v>
       </c>
       <c r="C545" s="3">
         <f>IF(EXACT(MAIN!$H545, ""), "", MAIN!$B545)</f>
@@ -31065,7 +31078,7 @@
       </c>
       <c r="F545" s="28" t="str">
         <f>IF(EXACT(MAIN!$H545, ""), "", ""&amp;MAIN!$E545)</f>
-        <v/>
+        <v>46000000000033</v>
       </c>
     </row>
     <row r="546" spans="2:6" x14ac:dyDescent="0.2">
@@ -31115,7 +31128,7 @@
     <row r="548" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B548" s="26">
         <f>IF(EXACT(MAIN!H548, ""), "", MAIN!G548)</f>
-        <v>225000000000031</v>
+        <v>225000000000032</v>
       </c>
       <c r="C548" s="3">
         <f>IF(EXACT(MAIN!$H548, ""), "", MAIN!$B548)</f>
@@ -31159,7 +31172,7 @@
     <row r="550" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B550" s="26">
         <f>IF(EXACT(MAIN!H550, ""), "", MAIN!G550)</f>
-        <v>225000000000032</v>
+        <v>225000000000033</v>
       </c>
       <c r="C550" s="3">
         <f>IF(EXACT(MAIN!$H550, ""), "", MAIN!$B550)</f>
@@ -31421,21 +31434,21 @@
       </c>
     </row>
     <row r="562" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B562" s="26" t="str">
+      <c r="B562" s="26">
         <f>IF(EXACT(MAIN!H562, ""), "", MAIN!G562)</f>
-        <v/>
-      </c>
-      <c r="C562" s="3" t="str">
+        <v>225000000000034</v>
+      </c>
+      <c r="C562" s="3">
         <f>IF(EXACT(MAIN!$H562, ""), "", MAIN!$B562)</f>
-        <v/>
+        <v>164000000000559</v>
       </c>
       <c r="D562" s="3" t="str">
         <f>IF(EXACT(MAIN!$H562, ""), "", MAIN!$C562)</f>
-        <v/>
-      </c>
-      <c r="E562" s="3" t="str">
+        <v>Adhe Kurniawan</v>
+      </c>
+      <c r="E562" s="3">
         <f>IF(EXACT(MAIN!$H562, ""), "", MAIN!$D562)</f>
-        <v/>
+        <v>95000000000015</v>
       </c>
       <c r="F562" s="28" t="str">
         <f>IF(EXACT(MAIN!$H562, ""), "", ""&amp;MAIN!$E562)</f>
@@ -31929,7 +31942,7 @@
     <row r="585" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B585" s="26">
         <f>IF(EXACT(MAIN!H585, ""), "", MAIN!G585)</f>
-        <v>225000000000033</v>
+        <v>225000000000035</v>
       </c>
       <c r="C585" s="3">
         <f>IF(EXACT(MAIN!$H585, ""), "", MAIN!$B585)</f>

</xml_diff>

<commit_message>
1. Update Excel SQL Generator 2. Pemasukan Programming/WebFrontEnd/storage/framework/sessions dalam Git
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblMapper_WorkerCareerInternalToUserRole.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblMapper_WorkerCareerInternalToUserRole.xlsx
@@ -386,7 +386,98 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6902,6 +6993,72 @@
           </cell>
           <cell r="M588" t="str">
             <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000585::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+          </cell>
+        </row>
+        <row r="589">
+          <cell r="C589" t="str">
+            <v>Budi Sandika</v>
+          </cell>
+          <cell r="L589">
+            <v>164000000000586</v>
+          </cell>
+          <cell r="M589" t="str">
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000586::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+          </cell>
+        </row>
+        <row r="590">
+          <cell r="C590" t="str">
+            <v>Fachri Azhar</v>
+          </cell>
+          <cell r="L590">
+            <v>164000000000587</v>
+          </cell>
+          <cell r="M590" t="str">
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, null::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+          </cell>
+        </row>
+        <row r="591">
+          <cell r="C591" t="str">
+            <v>Firmansyah Awaludin</v>
+          </cell>
+          <cell r="L591">
+            <v>164000000000588</v>
+          </cell>
+          <cell r="M591" t="str">
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, null::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+          </cell>
+        </row>
+        <row r="592">
+          <cell r="C592" t="str">
+            <v>Iman Faisal Abdurahman</v>
+          </cell>
+          <cell r="L592">
+            <v>164000000000589</v>
+          </cell>
+          <cell r="M592" t="str">
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, null::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+          </cell>
+        </row>
+        <row r="593">
+          <cell r="C593" t="str">
+            <v>Muhammad Irfan Alfikri</v>
+          </cell>
+          <cell r="L593">
+            <v>164000000000590</v>
+          </cell>
+          <cell r="M593" t="str">
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, null::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+          </cell>
+        </row>
+        <row r="594">
+          <cell r="C594" t="str">
+            <v>Syafri Johansah</v>
+          </cell>
+          <cell r="L594">
+            <v>164000000000591</v>
+          </cell>
+          <cell r="M594" t="str">
+            <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, null::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
           </cell>
         </row>
       </sheetData>
@@ -7201,14 +7358,14 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="B1:H589"/>
+  <dimension ref="B1:H594"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C341" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C579" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D230" sqref="D230"/>
       <selection pane="topRight" activeCell="D230" sqref="D230"/>
       <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
-      <selection pane="bottomRight" activeCell="C349" sqref="C349"/>
+      <selection pane="bottomRight" activeCell="H591" sqref="H591"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17816,7 +17973,7 @@
         <v>225000000000028</v>
       </c>
       <c r="H528" s="16" t="str">
-        <f t="shared" ref="H528:H589" si="18">IF(EXACT(D528, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B528, ""), "null", B528), "::bigint, ", IF(EXACT(D528, ""), "null", D528), "::bigint, ", IF(EXACT(E528, ""), "null", E528), "::bigint);"))</f>
+        <f t="shared" ref="H528:H591" si="18">IF(EXACT(D528, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B528, ""), "null", B528), "::bigint, ", IF(EXACT(D528, ""), "null", D528), "::bigint, ", IF(EXACT(E528, ""), "null", E528), "::bigint);"))</f>
         <v/>
       </c>
     </row>
@@ -18623,15 +18780,17 @@
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M568, ""), "", '[1]Internal Career (Last Position)'!$C568)</f>
         <v>Eka Kurniawan</v>
       </c>
-      <c r="D568" s="3"/>
+      <c r="D568" s="3">
+        <v>95000000000041</v>
+      </c>
       <c r="E568" s="3"/>
       <c r="G568" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H568" s="16" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblMapper_WorkerCareerInternalToUserRole_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 164000000000565::bigint, 95000000000041::bigint, null::bigint);</v>
       </c>
     </row>
     <row r="569" spans="2:8" x14ac:dyDescent="0.2">
@@ -18647,7 +18806,7 @@
       <c r="E569" s="3"/>
       <c r="G569" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H569" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18667,7 +18826,7 @@
       <c r="E570" s="3"/>
       <c r="G570" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H570" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18687,7 +18846,7 @@
       <c r="E571" s="3"/>
       <c r="G571" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H571" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18707,7 +18866,7 @@
       <c r="E572" s="3"/>
       <c r="G572" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H572" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18727,7 +18886,7 @@
       <c r="E573" s="3"/>
       <c r="G573" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H573" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18747,7 +18906,7 @@
       <c r="E574" s="3"/>
       <c r="G574" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H574" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18767,7 +18926,7 @@
       <c r="E575" s="3"/>
       <c r="G575" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H575" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18787,7 +18946,7 @@
       <c r="E576" s="3"/>
       <c r="G576" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H576" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18807,7 +18966,7 @@
       <c r="E577" s="3"/>
       <c r="G577" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H577" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18827,7 +18986,7 @@
       <c r="E578" s="3"/>
       <c r="G578" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H578" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18847,7 +19006,7 @@
       <c r="E579" s="3"/>
       <c r="G579" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H579" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18867,7 +19026,7 @@
       <c r="E580" s="3"/>
       <c r="G580" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H580" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18887,7 +19046,7 @@
       <c r="E581" s="3"/>
       <c r="G581" s="15">
         <f t="shared" si="17"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H581" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18906,8 +19065,8 @@
       <c r="D582" s="3"/>
       <c r="E582" s="3"/>
       <c r="G582" s="15">
-        <f t="shared" ref="G582:G589" si="19" xml:space="preserve"> G581 + IF(EXACT(H582, ""), 0, 1)</f>
-        <v>225000000000034</v>
+        <f t="shared" ref="G582:G593" si="19" xml:space="preserve"> G581 + IF(EXACT(H582, ""), 0, 1)</f>
+        <v>225000000000035</v>
       </c>
       <c r="H582" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18927,7 +19086,7 @@
       <c r="E583" s="3"/>
       <c r="G583" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H583" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18947,7 +19106,7 @@
       <c r="E584" s="3"/>
       <c r="G584" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000034</v>
+        <v>225000000000035</v>
       </c>
       <c r="H584" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18969,7 +19128,7 @@
       <c r="E585" s="3"/>
       <c r="G585" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000035</v>
+        <v>225000000000036</v>
       </c>
       <c r="H585" s="16" t="str">
         <f t="shared" si="18"/>
@@ -18989,7 +19148,7 @@
       <c r="E586" s="3"/>
       <c r="G586" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000035</v>
+        <v>225000000000036</v>
       </c>
       <c r="H586" s="16" t="str">
         <f t="shared" si="18"/>
@@ -19009,7 +19168,7 @@
       <c r="E587" s="3"/>
       <c r="G587" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000035</v>
+        <v>225000000000036</v>
       </c>
       <c r="H587" s="16" t="str">
         <f t="shared" si="18"/>
@@ -19029,7 +19188,7 @@
       <c r="E588" s="3"/>
       <c r="G588" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000035</v>
+        <v>225000000000036</v>
       </c>
       <c r="H588" s="16" t="str">
         <f t="shared" si="18"/>
@@ -19037,64 +19196,169 @@
       </c>
     </row>
     <row r="589" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B589" s="19" t="str">
+      <c r="B589" s="18">
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M589, ""), "", '[1]Internal Career (Last Position)'!$L589)</f>
-        <v/>
+        <v>164000000000586</v>
       </c>
       <c r="C589" s="18" t="str">
         <f>IF(EXACT('[1]Internal Career (Last Position)'!$M589, ""), "", '[1]Internal Career (Last Position)'!$C589)</f>
-        <v/>
-      </c>
-      <c r="D589" s="4"/>
-      <c r="E589" s="4"/>
+        <v>Budi Sandika</v>
+      </c>
+      <c r="D589" s="3"/>
+      <c r="E589" s="3"/>
       <c r="G589" s="15">
         <f t="shared" si="19"/>
-        <v>225000000000035</v>
-      </c>
-      <c r="H589" s="17" t="str">
+        <v>225000000000036</v>
+      </c>
+      <c r="H589" s="16" t="str">
         <f t="shared" si="18"/>
+        <v/>
+      </c>
+    </row>
+    <row r="590" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B590" s="18">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M590, ""), "", '[1]Internal Career (Last Position)'!$L590)</f>
+        <v>164000000000587</v>
+      </c>
+      <c r="C590" s="18" t="str">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M590, ""), "", '[1]Internal Career (Last Position)'!$C590)</f>
+        <v>Fachri Azhar</v>
+      </c>
+      <c r="D590" s="3"/>
+      <c r="E590" s="3"/>
+      <c r="G590" s="15">
+        <f t="shared" si="19"/>
+        <v>225000000000036</v>
+      </c>
+      <c r="H590" s="16" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+    </row>
+    <row r="591" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B591" s="18">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M591, ""), "", '[1]Internal Career (Last Position)'!$L591)</f>
+        <v>164000000000588</v>
+      </c>
+      <c r="C591" s="18" t="str">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M591, ""), "", '[1]Internal Career (Last Position)'!$C591)</f>
+        <v>Firmansyah Awaludin</v>
+      </c>
+      <c r="D591" s="3"/>
+      <c r="E591" s="3"/>
+      <c r="G591" s="15">
+        <f t="shared" si="19"/>
+        <v>225000000000036</v>
+      </c>
+      <c r="H591" s="16" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+    </row>
+    <row r="592" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B592" s="18">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M592, ""), "", '[1]Internal Career (Last Position)'!$L592)</f>
+        <v>164000000000589</v>
+      </c>
+      <c r="C592" s="18" t="str">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M592, ""), "", '[1]Internal Career (Last Position)'!$C592)</f>
+        <v>Iman Faisal Abdurahman</v>
+      </c>
+      <c r="D592" s="3"/>
+      <c r="E592" s="3"/>
+      <c r="G592" s="15">
+        <f t="shared" si="19"/>
+        <v>225000000000036</v>
+      </c>
+      <c r="H592" s="16" t="str">
+        <f t="shared" ref="H592:H593" si="20">IF(EXACT(D592, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B592, ""), "null", B592), "::bigint, ", IF(EXACT(D592, ""), "null", D592), "::bigint, ", IF(EXACT(E592, ""), "null", E592), "::bigint);"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="593" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B593" s="18">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M593, ""), "", '[1]Internal Career (Last Position)'!$L593)</f>
+        <v>164000000000590</v>
+      </c>
+      <c r="C593" s="18" t="str">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M593, ""), "", '[1]Internal Career (Last Position)'!$C593)</f>
+        <v>Muhammad Irfan Alfikri</v>
+      </c>
+      <c r="D593" s="3"/>
+      <c r="E593" s="3"/>
+      <c r="G593" s="15">
+        <f t="shared" si="19"/>
+        <v>225000000000036</v>
+      </c>
+      <c r="H593" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+    </row>
+    <row r="594" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B594" s="19">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M594, ""), "", '[1]Internal Career (Last Position)'!$L594)</f>
+        <v>164000000000591</v>
+      </c>
+      <c r="C594" s="19" t="str">
+        <f>IF(EXACT('[1]Internal Career (Last Position)'!$M594, ""), "", '[1]Internal Career (Last Position)'!$C594)</f>
+        <v>Syafri Johansah</v>
+      </c>
+      <c r="D594" s="4"/>
+      <c r="E594" s="4"/>
+      <c r="G594" s="15">
+        <f t="shared" ref="G590:G595" si="21" xml:space="preserve"> G593 + IF(EXACT(H594, ""), 0, 1)</f>
+        <v>225000000000036</v>
+      </c>
+      <c r="H594" s="17" t="str">
+        <f t="shared" ref="H590:H595" si="22">IF(EXACT(D594, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblMapper_WorkerCareerInternalToUserRole_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, ", IF(EXACT(B594, ""), "null", B594), "::bigint, ", IF(EXACT(D594, ""), "null", D594), "::bigint, ", IF(EXACT(E594, ""), "null", E594), "::bigint);"))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G12">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="20" priority="14">
       <formula>G11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="19" priority="13">
       <formula>G12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G18">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="18" priority="12">
       <formula>EXACT(G4, G5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>EXACT(G13, G14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>EXACT(G15, G16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G28">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>EXACT(G18, G19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G28">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>EXACT(G3, G4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G29:G589">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G29:G593">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>EXACT(G28, G29)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G594">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>EXACT(G593, G594)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31566,21 +31830,21 @@
       </c>
     </row>
     <row r="568" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B568" s="26" t="str">
+      <c r="B568" s="26">
         <f>IF(EXACT(MAIN!H568, ""), "", MAIN!G568)</f>
-        <v/>
-      </c>
-      <c r="C568" s="3" t="str">
+        <v>225000000000035</v>
+      </c>
+      <c r="C568" s="3">
         <f>IF(EXACT(MAIN!$H568, ""), "", MAIN!$B568)</f>
-        <v/>
+        <v>164000000000565</v>
       </c>
       <c r="D568" s="3" t="str">
         <f>IF(EXACT(MAIN!$H568, ""), "", MAIN!$C568)</f>
-        <v/>
-      </c>
-      <c r="E568" s="3" t="str">
+        <v>Eka Kurniawan</v>
+      </c>
+      <c r="E568" s="3">
         <f>IF(EXACT(MAIN!$H568, ""), "", MAIN!$D568)</f>
-        <v/>
+        <v>95000000000041</v>
       </c>
       <c r="F568" s="28" t="str">
         <f>IF(EXACT(MAIN!$H568, ""), "", ""&amp;MAIN!$E568)</f>
@@ -31942,7 +32206,7 @@
     <row r="585" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B585" s="26">
         <f>IF(EXACT(MAIN!H585, ""), "", MAIN!G585)</f>
-        <v>225000000000035</v>
+        <v>225000000000036</v>
       </c>
       <c r="C585" s="3">
         <f>IF(EXACT(MAIN!$H585, ""), "", MAIN!$B585)</f>

</xml_diff>